<commit_message>
Exercicios Funcoes Mercado de Trabalho
</commit_message>
<xml_diff>
--- a/5-FuncoesMercadoTrabalho/67. Função INDIRETO - Intervalos Nomeados - 1 - Material(1).xlsx
+++ b/5-FuncoesMercadoTrabalho/67. Função INDIRETO - Intervalos Nomeados - 1 - Material(1).xlsx
@@ -1,20 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaof\Desktop\Excel Impressionador 2021\Módulo 8 - Funções Mercado de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cursos\excel\5-FuncoesMercadoTrabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C38312D-CE8D-4339-BCB9-83F5508DBD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0441A45-3077-4703-9A16-E7D1FCAF905B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="801" xr2:uid="{C3784EBB-09BF-477B-9CB0-C14E8EE5D46B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="801" xr2:uid="{C3784EBB-09BF-477B-9CB0-C14E8EE5D46B}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="23" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Ano_2010">Base!$C$3:$I$3</definedName>
+    <definedName name="Ano_2011">Base!$C$4:$I$4</definedName>
+    <definedName name="Ano_2012">Base!$C$5:$I$5</definedName>
+    <definedName name="Ano_2013">Base!$C$6:$I$6</definedName>
+    <definedName name="Ano_2014">Base!$C$7:$I$7</definedName>
+    <definedName name="Ano_2015">Base!$C$8:$I$8</definedName>
+    <definedName name="Ano_2016">Base!$C$9:$I$9</definedName>
+    <definedName name="Ano_2017">Base!$C$10:$I$10</definedName>
+    <definedName name="Ano_2018">Base!$C$11:$I$11</definedName>
+    <definedName name="Ano_2019">Base!$C$12:$I$12</definedName>
+    <definedName name="Ano_2020">Base!$C$13:$I$13</definedName>
+    <definedName name="Corolla">Base!$E$3:$E$13</definedName>
+    <definedName name="Duster">Base!$G$3:$G$13</definedName>
+    <definedName name="Etios">Base!$F$3:$F$13</definedName>
+    <definedName name="Kicks">Base!$D$3:$D$13</definedName>
+    <definedName name="Logan">Base!$H$3:$H$13</definedName>
+    <definedName name="Sandero">Base!$I$3:$I$13</definedName>
+    <definedName name="Versa">Base!$C$3:$C$13</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,12 +49,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Produção</t>
   </si>
@@ -79,6 +102,39 @@
   </si>
   <si>
     <t>Marca</t>
+  </si>
+  <si>
+    <t>Ano_2010</t>
+  </si>
+  <si>
+    <t>Ano_2011</t>
+  </si>
+  <si>
+    <t>Ano_2012</t>
+  </si>
+  <si>
+    <t>Ano_2013</t>
+  </si>
+  <si>
+    <t>Ano_2014</t>
+  </si>
+  <si>
+    <t>Ano_2015</t>
+  </si>
+  <si>
+    <t>Ano_2016</t>
+  </si>
+  <si>
+    <t>Ano_2017</t>
+  </si>
+  <si>
+    <t>Ano_2018</t>
+  </si>
+  <si>
+    <t>Ano_2019</t>
+  </si>
+  <si>
+    <t>Ano_2020</t>
   </si>
 </sst>
 </file>
@@ -178,9 +234,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -218,7 +274,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -324,7 +380,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,7 +522,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -477,17 +533,19 @@
   <dimension ref="B2:M13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="9" width="10.88671875" customWidth="1"/>
-    <col min="11" max="13" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="9" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -513,7 +571,7 @@
         <v>11</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>0</v>
@@ -522,9 +580,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="5">
-        <v>2010</v>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C3" s="3">
         <v>73400</v>
@@ -550,14 +608,17 @@
       <c r="K3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="3"/>
+      <c r="L3" s="3">
+        <f ca="1">SUM(INDIRECT(K2))</f>
+        <v>601700</v>
+      </c>
       <c r="M3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
-        <v>2011</v>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="C4" s="3">
         <v>73100</v>
@@ -583,14 +644,15 @@
       <c r="K4" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
-        <v>2012</v>
+      <c r="L4" s="3">
+        <f ca="1">AVERAGE(INDIRECT(K2))</f>
+        <v>54700</v>
+      </c>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="C5" s="3">
         <v>97000</v>
@@ -616,12 +678,18 @@
       <c r="K5" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="5">
-        <v>2013</v>
+      <c r="L5" s="3">
+        <f ca="1">MAX(INDIRECT(K2))</f>
+        <v>82800</v>
+      </c>
+      <c r="M5" s="7" t="str">
+        <f ca="1">INDEX(B3:B13, MATCH(L5, INDIRECT(K2), 0))</f>
+        <v>Ano_2016</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="C6" s="3">
         <v>88500</v>
@@ -647,12 +715,18 @@
       <c r="K6" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="5">
-        <v>2014</v>
+      <c r="L6" s="3">
+        <f ca="1">MIN(INDIRECT(K2))</f>
+        <v>10500</v>
+      </c>
+      <c r="M6" s="7" t="str">
+        <f ca="1">INDEX(B3:B13, MATCH(L6, INDIRECT(K2),0))</f>
+        <v>Ano_2018</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C7" s="3">
         <v>83600</v>
@@ -676,9 +750,9 @@
         <v>76500</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="5">
-        <v>2015</v>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C8" s="3">
         <v>43800</v>
@@ -701,8 +775,8 @@
       <c r="I8" s="3">
         <v>59800</v>
       </c>
-      <c r="K8" s="1">
-        <v>2014</v>
+      <c r="K8" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>0</v>
@@ -711,9 +785,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="5">
-        <v>2016</v>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="3">
         <v>25300</v>
@@ -739,14 +813,17 @@
       <c r="K9" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="3"/>
+      <c r="L9" s="3">
+        <f ca="1">SUM(INDIRECT(K8))</f>
+        <v>359900</v>
+      </c>
       <c r="M9" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="5">
-        <v>2017</v>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="C10" s="3">
         <v>16000</v>
@@ -772,14 +849,17 @@
       <c r="K10" t="s">
         <v>2</v>
       </c>
-      <c r="L10" s="3"/>
+      <c r="L10" s="3">
+        <f ca="1">AVERAGE(INDIRECT(K8))</f>
+        <v>51414.285714285717</v>
+      </c>
       <c r="M10" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="5">
-        <v>2018</v>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C11" s="3">
         <v>60900</v>
@@ -805,12 +885,18 @@
       <c r="K11" t="s">
         <v>3</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="7"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="5">
-        <v>2019</v>
+      <c r="L11" s="3">
+        <f ca="1">MAX(INDIRECT(K8))</f>
+        <v>87900</v>
+      </c>
+      <c r="M11" s="7" t="str">
+        <f ca="1">INDEX(C2:I2, MATCH(L11, INDIRECT(K8), 0))</f>
+        <v>Versa</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C12" s="3">
         <v>36000</v>
@@ -836,12 +922,18 @@
       <c r="K12" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="7"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="5">
-        <v>2020</v>
+      <c r="L12" s="3">
+        <f ca="1">MIN(INDIRECT(K8))</f>
+        <v>17700</v>
+      </c>
+      <c r="M12" s="7" t="str">
+        <f ca="1">INDEX(C2:I2, MATCH(L12, INDIRECT(K8), 0))</f>
+        <v>Etios</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C13" s="3">
         <v>87900</v>

</xml_diff>